<commit_message>
Correct y-axis label of HERG count graph
</commit_message>
<xml_diff>
--- a/data/thievingHERGnotes.xlsx
+++ b/data/thievingHERGnotes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marina\Desktop\Repositories\thieving-HERGs-2024\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0ED50EE2-2133-4E2F-9F40-20D2B180A68E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FE79A7-E94B-4DC5-9D5B-522A69EF7EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-75" yWindow="0" windowWidth="9750" windowHeight="10155" activeTab="2" xr2:uid="{A0112574-F2AE-4111-A3FF-2AF6F55EEE7B}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{A0112574-F2AE-4111-A3FF-2AF6F55EEE7B}"/>
   </bookViews>
   <sheets>
     <sheet name="environment" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,9 @@
     <sheet name="outtakes" sheetId="5" r:id="rId4"/>
     <sheet name="codebook" sheetId="3" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">observations!$A$1:$T$70</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -953,7 +956,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B12A18-ED9C-425B-8F32-89341C7D0343}">
   <dimension ref="A1:S13"/>
   <sheetViews>
-    <sheetView zoomScale="81" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
       <selection activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
@@ -1791,9 +1794,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD06F2EE-F4A2-49D9-B434-4B6E37D81E4C}">
   <dimension ref="A1:T70"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T71" sqref="T71"/>
+    <sheetView zoomScale="65" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6155,6 +6158,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:T70" xr:uid="{DD06F2EE-F4A2-49D9-B434-4B6E37D81E4C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -6164,7 +6168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A64EF174-6894-4D77-84AF-89E54ED24D01}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>